<commit_message>
Fin du HSIS_ApaliPi Suppression de l'exemple
</commit_message>
<xml_diff>
--- a/ApaliPi-config-1.xlsx
+++ b/ApaliPi-config-1.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_7D32F16947DEEC44FB1DC1CB46AF5B4A5438CCC7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB403CF5-5F22-4D99-8692-5279316B74A8}"/>
+  <bookViews>
+    <workbookView xWindow="345" yWindow="345" windowWidth="16605" windowHeight="13755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Pin Configuration" state="visible" r:id="rId4"/>
+    <sheet name="Pin Configuration" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="233">
   <si>
     <t>Signal</t>
   </si>
@@ -707,31 +711,40 @@
   </si>
   <si>
     <t>USB3_DN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial Black"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE7AD0E"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <name val="Arial Black"/>
-    </font>
-    <font>
-      <color rgb="FFE7AD0E"/>
-    </font>
-    <font>
+      <sz val="11"/>
       <color rgb="FF27BD4B"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -769,10 +782,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1152,12 +1173,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <tabColor rgb="FFC0000"/>
+    <tabColor rgb="FFFC0000"/>
   </sheetPr>
-  <dimension ref="A1:J64"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <dimension ref="A1:K64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
@@ -1171,7 +1197,7 @@
     <col min="10" max="10" width="27" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1203,7 +1229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1232,7 +1258,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -1261,7 +1287,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -1290,7 +1316,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
@@ -1319,7 +1345,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
@@ -1348,7 +1374,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
@@ -1377,7 +1403,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
@@ -1406,7 +1432,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1435,7 +1461,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
@@ -1464,7 +1490,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>40</v>
       </c>
@@ -1493,7 +1519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>43</v>
       </c>
@@ -1522,7 +1548,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -1551,7 +1577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>54</v>
       </c>
@@ -1580,7 +1606,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>57</v>
       </c>
@@ -1609,7 +1635,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>60</v>
       </c>
@@ -1638,7 +1664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>63</v>
       </c>
@@ -1667,7 +1693,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>66</v>
       </c>
@@ -1696,7 +1722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>69</v>
       </c>
@@ -1725,7 +1751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>72</v>
       </c>
@@ -1754,7 +1780,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>77</v>
       </c>
@@ -1783,7 +1809,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>80</v>
       </c>
@@ -1812,7 +1838,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>83</v>
       </c>
@@ -1841,7 +1867,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>86</v>
       </c>
@@ -1870,7 +1896,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>89</v>
       </c>
@@ -1899,7 +1925,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>92</v>
       </c>
@@ -1928,7 +1954,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>95</v>
       </c>
@@ -1957,7 +1983,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>98</v>
       </c>
@@ -1986,7 +2012,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>101</v>
       </c>
@@ -2015,7 +2041,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>104</v>
       </c>
@@ -2044,7 +2070,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>107</v>
       </c>
@@ -2073,7 +2099,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>111</v>
       </c>
@@ -2102,7 +2128,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>115</v>
       </c>
@@ -2131,7 +2157,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>118</v>
       </c>
@@ -2160,7 +2186,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>121</v>
       </c>
@@ -2189,7 +2215,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>124</v>
       </c>
@@ -2218,7 +2244,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>127</v>
       </c>
@@ -2247,7 +2273,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>130</v>
       </c>
@@ -2276,7 +2302,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>133</v>
       </c>
@@ -2305,7 +2331,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>136</v>
       </c>
@@ -2334,7 +2360,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>139</v>
       </c>
@@ -2363,7 +2389,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>143</v>
       </c>
@@ -2392,7 +2418,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>147</v>
       </c>
@@ -2420,8 +2446,11 @@
       <c r="J43" s="13" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K43" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>151</v>
       </c>
@@ -2450,7 +2479,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>155</v>
       </c>
@@ -2479,7 +2508,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>159</v>
       </c>
@@ -2508,7 +2537,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>163</v>
       </c>
@@ -2537,7 +2566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>167</v>
       </c>
@@ -2566,7 +2595,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>171</v>
       </c>
@@ -2595,7 +2624,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>175</v>
       </c>
@@ -2624,7 +2653,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>179</v>
       </c>
@@ -2653,7 +2682,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>183</v>
       </c>
@@ -2682,7 +2711,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>187</v>
       </c>
@@ -2711,7 +2740,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>192</v>
       </c>
@@ -2740,7 +2769,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>196</v>
       </c>
@@ -2769,7 +2798,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>200</v>
       </c>
@@ -2798,7 +2827,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>204</v>
       </c>
@@ -2827,7 +2856,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>208</v>
       </c>
@@ -2856,7 +2885,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>212</v>
       </c>
@@ -2885,7 +2914,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>216</v>
       </c>
@@ -2914,7 +2943,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>220</v>
       </c>
@@ -2943,7 +2972,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>223</v>
       </c>
@@ -2972,7 +3001,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>226</v>
       </c>
@@ -3001,7 +3030,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>229</v>
       </c>
@@ -3032,6 +3061,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>